<commit_message>
Merged PR 1710: Task 335717: Багфикс TLC
</commit_message>
<xml_diff>
--- a/Module.Frontend.TPM/Content/Templates/TLCClosedTemplate.xlsx
+++ b/Module.Frontend.TPM/Content/Templates/TLCClosedTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windows\Temp\TPM\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\TPM\Module.Frontend.TPM\Content\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E83062-3B64-42BC-B0E4-FA2DEF2950E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C254E9-2BB5-45C7-9DB6-861E0A9D9E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="134">
   <si>
     <t>Promo Type</t>
   </si>
@@ -447,15 +447,6 @@
   </si>
   <si>
     <t>85g</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>TPR</t>
-  </si>
-  <si>
-    <t>VP</t>
   </si>
 </sst>
 </file>
@@ -6816,26 +6807,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC80930-7F4F-4A05-A0B9-C5579139E38B}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6880,15 +6863,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008BD6AFE2CAF68846A90AF41F02AA6078" ma:contentTypeVersion="50" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d98a57736acbe81ebd48d911a51b45cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="583145ed-b998-4802-bdfd-b0ec64ffe47d" xmlns:ns3="e45562e1-71fb-4bba-8dff-84d3788fc1cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57b2f41c826d6401cab8db36b557d145" ns2:_="" ns3:_="">
     <xsd:import namespace="583145ed-b998-4802-bdfd-b0ec64ffe47d"/>
@@ -7127,15 +7101,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22864964-7C3A-4ABB-9D0F-1C39BEC70B4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AB4ACE0-426F-47A4-8AC8-CF7B3D89BA26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7152,4 +7127,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22864964-7C3A-4ABB-9D0F-1C39BEC70B4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>